<commit_message>
output now detects completed and uncompleted courses and outputs them to Excel
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -451,12 +451,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Course Names</t>
+          <t>Completed Courses</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Completed Dts</t>
+          <t>Uncompleted Courses</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[Timestamp('2024-08-31 00:00:00'), Timestamp('2024-08-31 00:00:00'), Timestamp('2024-08-31 00:00:00')]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -507,12 +507,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)', 'Supervisor Safety Training (2 hrs)', 'Employee Safety (1 hr)']</t>
+          <t>['Supervisor Safety Training (2 hrs)', 'Employee Safety (1 hr)']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[Timestamp('2024-08-30 00:00:00'), Timestamp('2024-08-30 00:00:00'), Timestamp('2024-08-30 00:00:00'), Timestamp('2024-08-29 00:00:00')]</t>
+          <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)']</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[Timestamp('2024-08-29 00:00:00'), Timestamp('2024-08-29 00:00:00'), Timestamp('2024-08-29 00:00:00'), Timestamp('2024-08-28 00:00:00')]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -568,7 +568,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[Timestamp('2024-08-28 00:00:00'), Timestamp('2024-08-28 00:00:00'), Timestamp('2024-08-28 00:00:00'), Timestamp('2024-08-28 00:00:00')]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
separate first and last names
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Completed Courses</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Uncompleted Courses</t>
         </is>
@@ -469,20 +474,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>John</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>ACTIVE DUTY</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)', 'Supervisor Safety Training (2 hrs)']</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -497,20 +507,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Andrew Hartmann</t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Hartmann</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>DOD CIVILLIAN</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>['Supervisor Safety Training (2 hrs)', 'Employee Safety (1 hr)']</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)']</t>
         </is>
@@ -525,20 +540,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nick Fletcher</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Fletcher</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>DOD CIVILLIAN</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)', 'Supervisor Safety Training (2 hrs)', 'Employee Safety (1 hr)']</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -553,20 +573,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>John Cena</t>
+          <t>John</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>ACTIVE DUTY</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>['DHA Accommodations (1 hr)', 'Leadership Training (4 hrs)', 'MHS Customer Service (1 hr)', 'Violence Response (1 hr)']</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
output more closely resembles expected output
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,42 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Completed Courses</t>
+          <t>DHA Accommodations (1 hr)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Uncompleted Courses</t>
+          <t>Leadership Training (4 hrs)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MHS Customer Service (1 hr)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Counterintelligence (1 hr)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>HIPAA Training (1 hr)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Supervisor Safety Training (2 hrs)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Employee Safety (1 hr)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Violence Response (1 hr)</t>
         </is>
       </c>
     </row>
@@ -489,14 +519,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)', 'Supervisor Safety Training (2 hrs)']</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -520,16 +560,30 @@
           <t>DOD CIVILLIAN</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>['Supervisor Safety Training (2 hrs)', 'Employee Safety (1 hr)']</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)']</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NOT Completed</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NOT Completed</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -553,16 +607,30 @@
           <t>DOD CIVILLIAN</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>['Counterintelligence (1 hr)', 'HIPAA Training (1 hr)', 'Supervisor Safety Training (2 hrs)', 'Employee Safety (1 hr)']</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -588,12 +656,26 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['DHA Accommodations (1 hr)', 'Leadership Training (4 hrs)', 'MHS Customer Service (1 hr)', 'Violence Response (1 hr)']</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Completed</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
use column indeces from sources.csv instead of hard coded
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,45 +451,40 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>DHA Accommodations (1 hr)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>DHA Accommodations (1 hr)</t>
+          <t>Leadership Training (4 hrs)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Leadership Training (4 hrs)</t>
+          <t>MHS Customer Service (1 hr)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>MHS Customer Service (1 hr)</t>
+          <t>Counterintelligence (1 hr)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Counterintelligence (1 hr)</t>
+          <t>HIPAA Training (1 hr)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>HIPAA Training (1 hr)</t>
+          <t>Supervisor Safety Training (2 hrs)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Supervisor Safety Training (2 hrs)</t>
+          <t>Employee Safety (1 hr)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Employee Safety (1 hr)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Violence Response (1 hr)</t>
         </is>
@@ -514,7 +509,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ACTIVE DUTY</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -527,16 +522,11 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -555,14 +545,14 @@
           <t>Hartmann</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DOD CIVILLIAN</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NOT Completed</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>NOT Completed</t>
@@ -570,7 +560,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NOT Completed</t>
+          <t>LATE (completed)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -578,12 +568,7 @@
           <t>LATE (completed)</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -602,14 +587,14 @@
           <t>Fletcher</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>DOD CIVILLIAN</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>Completed</t>
@@ -617,7 +602,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>LATE (completed)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -625,12 +610,7 @@
           <t>LATE (completed)</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -651,7 +631,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ACTIVE DUTY</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -664,16 +644,11 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>

</xml_diff>

<commit_message>
fixed course name parsing
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,60 +434,26 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>EDIPI</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>DHA Accommodations (1 hr)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Leadership Training (4 hrs)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>MHS Customer Service (1 hr)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Counterintelligence (1 hr)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>HIPAA Training (1 hr)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Supervisor Safety Training (2 hrs)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Employee Safety (1 hr)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Violence Response (1 hr)</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1234567891</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>3322111234</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4453245321</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>5555555555</v>
       </c>
     </row>
     <row r="2">
@@ -512,21 +478,9 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -546,29 +500,13 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>LATE (completed)</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>NOT Completed</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>NOT Completed</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -579,7 +517,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Nicholas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -589,28 +527,12 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -621,7 +543,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>J</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -629,28 +551,12 @@
           <t>Cena</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Completed</t>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>LATE (completed)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed JKO source data
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,17 +443,45 @@
       <c r="D1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>1234567891</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>3322111234</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>4453245321</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>5555555555</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>DHA Accommodations (1 hr)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Leadership Training (4 hrs)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MHS Customer Service (1 hr)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Counterintelligence (1 hr)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>HIPAA Training (1 hr)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Supervisor Safety Training (2 hrs)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Employee Safety (1 hr)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>RandomCourse</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -478,9 +506,21 @@
           <t>Completed</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -500,13 +540,29 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NOT Completed</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NOT Completed</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>LATE (completed)</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>LATE (completed)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -527,12 +583,16 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -554,7 +614,11 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
         <is>
           <t>LATE (completed)</t>
         </is>

</xml_diff>

<commit_message>
parses by email if no ID is present
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,45 +445,40 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>DHA Accommodations (1 hr)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Leadership Training (4 hrs)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MHS Customer Service (1 hr)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Counterintelligence (1 hr)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>HIPAA Training (1 hr)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Supervisor Safety Training (2 hrs)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Employee Safety (1 hr)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>DHA Accommodations (1 hr)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Leadership Training (4 hrs)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>MHS Customer Service (1 hr)</t>
-        </is>
-      </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Violence Response (1 hr)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>RandomCourse</t>
         </is>
@@ -493,183 +488,139 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>andrewh@myspace.com</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1234567891</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>John</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hartmann</t>
+          <t>Doe</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NOT Completed</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NOT Completed</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>john.cena@gmail.com</t>
-        </is>
+      <c r="B3" t="n">
+        <v>3322111234</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Hartmann</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NOT Completed</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>NOT Completed</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>LATE (completed)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
           <t>LATE (completed)</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>johndoe@email.com</t>
-        </is>
+      <c r="B4" t="n">
+        <v>4453245321</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Nicholas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Doe</t>
+          <t>Fletcher</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>nfeltcher@yahoo.com</t>
-        </is>
+      <c r="B5" t="n">
+        <v>5555555555</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>J</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fletcher</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Completed</t>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>LATE (completed)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add courses to id builder
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,53 +438,74 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>0</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dodid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>cleanName</t>
+        </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>DHA Accommodations (1 hr)</t>
+          <t>fullName</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Leadership Training (4 hrs)</t>
+          <t>courseName</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>MHS Customer Service (1 hr)</t>
+          <t>DHA Accommodations (1 hr)-JKO</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Counterintelligence (1 hr)</t>
+          <t>Leadership Training (4 hrs)-JKO</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>HIPAA Training (1 hr)</t>
+          <t>MHS Customer Service (1 hr)-JKO</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Supervisor Safety Training (2 hrs)</t>
+          <t>Counterintelligence (1 hr)-JKO</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Employee Safety (1 hr)</t>
+          <t>HIPAA Training (1 hr)-JKO</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>RandomCourse</t>
+          <t>Supervisor Safety Training (2 hrs)-JKO</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Employee Safety (1 hr)-JKO</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Violence Response (1 hr)-JKO</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>RandomCourse-JKO</t>
         </is>
       </c>
     </row>
@@ -491,36 +516,33 @@
       <c r="B2" t="n">
         <v>1234567891</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Doe</t>
+          <t>johndoe</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45536</v>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -529,40 +551,35 @@
       <c r="B3" t="n">
         <v>3322111234</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hartmann</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>andrewhartmann</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Andrew Hartmann</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>NOT Completed</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>NOT Completed</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -571,27 +588,36 @@
       <c r="B4" t="n">
         <v>4453245321</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Nicholas</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fletcher</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>nickfletcher</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Nick Fletcher</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
+      <c r="J4" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" s="2" t="n">
+        <v>36527</v>
       </c>
     </row>
     <row r="5">
@@ -601,27 +627,36 @@
       <c r="B5" t="n">
         <v>5555555555</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cena</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>johncena</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>John Cena</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="G5" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>45536</v>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>LATE (completed)</t>
-        </is>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" s="2" t="n">
+        <v>45536</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>36161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix name match happening for different id people
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,47 +460,47 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>DHA Accommodations (1 hr)-missingID</t>
+          <t>DHA Accommodations (1 hr)-JKO</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Leadership Training (4 hrs)-missingID</t>
+          <t>Leadership Training (4 hrs)-JKO</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>MHS Customer Service (1 hr)-missingID</t>
+          <t>MHS Customer Service (1 hr)-JKO</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Counterintelligence (1 hr)-missingID</t>
+          <t>Counterintelligence (1 hr)-JKO</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>HIPAA Training (1 hr)-missingID</t>
+          <t>HIPAA Training (1 hr)-JKO</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Supervisor Safety Training (2 hrs)-missingID</t>
+          <t>Supervisor Safety Training (2 hrs)-JKO</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Employee Safety (1 hr)-missingID</t>
+          <t>Employee Safety (1 hr)-JKO</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Violence Response (1 hr)-missingID</t>
+          <t>Violence Response (1 hr)-JKO</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>RandomCourse-missingID</t>
+          <t>RandomCourse-JKO</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -541,51 +541,6 @@
       <c r="U1" s="1" t="inlineStr">
         <is>
           <t>RandomCourseName2-myLearning</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>DHA Accommodations (1 hr)-JKO</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Leadership Training (4 hrs)-JKO</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>MHS Customer Service (1 hr)-JKO</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Counterintelligence (1 hr)-JKO</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>HIPAA Training (1 hr)-JKO</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Supervisor Safety Training (2 hrs)-JKO</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Employee Safety (1 hr)-JKO</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Violence Response (1 hr)-JKO</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>RandomCourse-JKO</t>
         </is>
       </c>
     </row>
@@ -593,11 +548,7 @@
       <c r="A2" t="n">
         <v>1234567891</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>johndoe@email.com</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>johndoe</t>
@@ -631,31 +582,12 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="W2" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="X2" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>3322111234</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>andrewh@myspace.com</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>andrewhartmann</t>
@@ -691,23 +623,6 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="Z3" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="AA3" s="2" t="n">
-        <v>45505</v>
-      </c>
-      <c r="AB3" s="2" t="n">
-        <v>45505</v>
-      </c>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -715,7 +630,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>nfeltcher@yahoo.com</t>
+          <t>n@gmail.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -757,35 +672,12 @@
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="Z4" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="AA4" s="2" t="n">
-        <v>45505</v>
-      </c>
-      <c r="AB4" s="2" t="n">
-        <v>45505</v>
-      </c>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" s="2" t="n">
-        <v>36527</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>5555555555</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>john.cena@gmail.com</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>johncena</t>
@@ -823,25 +715,6 @@
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
-      <c r="V5" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="W5" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="X5" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="AD5" s="2" t="n">
-        <v>36161</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -883,15 +756,6 @@
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -929,15 +793,6 @@
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -973,15 +828,6 @@
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1017,15 +863,6 @@
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1061,15 +898,6 @@
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1105,15 +933,6 @@
         <v>44326</v>
       </c>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1149,15 +968,6 @@
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1193,15 +1003,6 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1237,15 +1038,6 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1281,15 +1073,6 @@
       <c r="U15" s="2" t="n">
         <v>45222</v>
       </c>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
progress on output coloring
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>dodid</t>
   </si>
@@ -28,106 +28,61 @@
     <t>fullName</t>
   </si>
   <si>
-    <t>Survival-myLearning</t>
-  </si>
-  <si>
-    <t>Swimming-myLearning</t>
-  </si>
-  <si>
-    <t>Flying-myLearning</t>
-  </si>
-  <si>
-    <t>Electronics-myLearning</t>
-  </si>
-  <si>
-    <t>RandomCourseName-myLearning</t>
-  </si>
-  <si>
-    <t>Cooking-myLearning</t>
-  </si>
-  <si>
-    <t>Navigation-myLearning</t>
-  </si>
-  <si>
-    <t>RandomCourseName2-myLearning</t>
-  </si>
-  <si>
-    <t>n@gmail.com</t>
-  </si>
-  <si>
-    <t>nicholasfletcher</t>
-  </si>
-  <si>
-    <t>sallysmith</t>
-  </si>
-  <si>
-    <t>bobcole</t>
-  </si>
-  <si>
-    <t>daviddun</t>
-  </si>
-  <si>
-    <t>emilydonald</t>
-  </si>
-  <si>
-    <t>billblah</t>
-  </si>
-  <si>
-    <t>cliftondonald</t>
-  </si>
-  <si>
-    <t>nancybryan</t>
-  </si>
-  <si>
-    <t>nevinfish</t>
-  </si>
-  <si>
-    <t>laracronin</t>
-  </si>
-  <si>
-    <t>camyrnmoltavo</t>
-  </si>
-  <si>
-    <t>Nicholas Fletcher</t>
-  </si>
-  <si>
-    <t>Sally Smith</t>
-  </si>
-  <si>
-    <t>Bob Cole</t>
-  </si>
-  <si>
-    <t>David Dun</t>
-  </si>
-  <si>
-    <t>Emily Donald</t>
-  </si>
-  <si>
-    <t>Bill Blah</t>
-  </si>
-  <si>
-    <t>Clifton Donald</t>
-  </si>
-  <si>
-    <t>Nancy Bryan</t>
-  </si>
-  <si>
-    <t>Nevin Fish</t>
-  </si>
-  <si>
-    <t>Lara Cronin</t>
-  </si>
-  <si>
-    <t>Camyrn Moltavo</t>
+    <t>DHA Accommodations (1 hr)-JKO</t>
+  </si>
+  <si>
+    <t>Leadership Training (4 hrs)-JKO</t>
+  </si>
+  <si>
+    <t>MHS Customer Service (1 hr)-JKO</t>
+  </si>
+  <si>
+    <t>Counterintelligence (1 hr)-JKO</t>
+  </si>
+  <si>
+    <t>HIPAA Training (1 hr)-JKO</t>
+  </si>
+  <si>
+    <t>Supervisor Safety Training (2 hrs)-JKO</t>
+  </si>
+  <si>
+    <t>Employee Safety (1 hr)-JKO</t>
+  </si>
+  <si>
+    <t>Violence Response (1 hr)-JKO</t>
+  </si>
+  <si>
+    <t>RandomCourse-JKO</t>
+  </si>
+  <si>
+    <t>johndoe</t>
+  </si>
+  <si>
+    <t>andrewhartmann</t>
+  </si>
+  <si>
+    <t>nickfletcher</t>
+  </si>
+  <si>
+    <t>johncena</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Andrew Hartmann</t>
+  </si>
+  <si>
+    <t>Nick Fletcher</t>
+  </si>
+  <si>
+    <t>John Cena</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -186,22 +141,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF000000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -209,6 +170,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC0C0C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -502,17 +470,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="13" width="30.7109375" customWidth="1"/>
+    <col min="5" max="14" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -549,185 +517,171 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
-        <v>4453245321</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>1234567891</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3">
-        <v>44836</v>
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>3322111234</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3">
-        <v>44019</v>
-      </c>
-      <c r="F3" s="3">
-        <v>44197</v>
-      </c>
-      <c r="G3" s="3">
-        <v>43863</v>
-      </c>
-      <c r="J3" s="3">
-        <v>45577</v>
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>CHOOSE(1,"2024-08-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>CHOOSE(1,"2024-08-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>4453245321</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3">
-        <v>43685</v>
-      </c>
-      <c r="G4" s="3">
-        <v>45185</v>
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>CHOOSE(1,"2024-08-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>CHOOSE(1,"2024-08-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>CHOOSE(1,"2000-01-02 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>5555555555</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1">
-        <v>55</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="3">
-        <v>45650</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1">
-        <v>100</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="3">
-        <v>45386</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="3">
-        <v>44326</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="3">
-        <v>45058</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="3">
-        <v>45463</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1">
-        <v>40</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="3">
-        <v>44478</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1">
-        <v>80</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="3">
-        <v>45222</v>
+      <c r="E5">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>CHOOSE(1,"2024-09-01 00:00:00","('IND_ONTIME',)")</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>CHOOSE(1,"1999-01-01 00:00:00","('IND_OVERDUE',)")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A12:L13">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A12))=0</formula>
+  <conditionalFormatting sqref="E2:M4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISNUMBER(SEARCH("('IND_OVERDUE',)", _xlfn.FORMULATEXT(E2)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:L11">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(E2))=0</formula>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISNUMBER(SEARCH("('IND_ONTIME',)", _xlfn.FORMULATEXT(E2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>ISNUMBER(SEARCH("IND_NOTASSIGNED", _xlfn.FORMULATEXT(E2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISNUMBER(SEARCH("('IND_ASSIGNED',)", _xlfn.FORMULATEXT(E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished logging and some bug fixes
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>dodid</t>
   </si>
@@ -55,6 +55,96 @@
     <t>RandomCourse-JKO</t>
   </si>
   <si>
+    <t>Survival-myLearning</t>
+  </si>
+  <si>
+    <t>Swimming-myLearning</t>
+  </si>
+  <si>
+    <t>Flying-myLearning</t>
+  </si>
+  <si>
+    <t>Electronics-myLearning</t>
+  </si>
+  <si>
+    <t>RandomCourseName-myLearning</t>
+  </si>
+  <si>
+    <t>Cooking-myLearning</t>
+  </si>
+  <si>
+    <t>Navigation-myLearning</t>
+  </si>
+  <si>
+    <t>RandomCourseName2-myLearning</t>
+  </si>
+  <si>
+    <t>DHA Accommodations (1 hr)-badSource</t>
+  </si>
+  <si>
+    <t>Leadership Training (4 hrs)-badSource</t>
+  </si>
+  <si>
+    <t>MHS Customer Service (1 hr)-badSource</t>
+  </si>
+  <si>
+    <t>Counterintelligence (1 hr)-badSource</t>
+  </si>
+  <si>
+    <t>HIPAA Training (1 hr)-badSource</t>
+  </si>
+  <si>
+    <t>Supervisor Safety Training (2 hrs)-badSource</t>
+  </si>
+  <si>
+    <t>Employee Safety (1 hr)-badSource</t>
+  </si>
+  <si>
+    <t>Violence Response (1 hr)-badSource</t>
+  </si>
+  <si>
+    <t>RandomCourse-badSource</t>
+  </si>
+  <si>
+    <t>DHA Accommodations (1 hr)-missingID</t>
+  </si>
+  <si>
+    <t>Leadership Training (4 hrs)-missingID</t>
+  </si>
+  <si>
+    <t>MHS Customer Service (1 hr)-missingID</t>
+  </si>
+  <si>
+    <t>Counterintelligence (1 hr)-missingID</t>
+  </si>
+  <si>
+    <t>HIPAA Training (1 hr)-missingID</t>
+  </si>
+  <si>
+    <t>Supervisor Safety Training (2 hrs)-missingID</t>
+  </si>
+  <si>
+    <t>Employee Safety (1 hr)-missingID</t>
+  </si>
+  <si>
+    <t>Violence Response (1 hr)-missingID</t>
+  </si>
+  <si>
+    <t>RandomCourse-missingID</t>
+  </si>
+  <si>
+    <t>johndoe@email.com</t>
+  </si>
+  <si>
+    <t>andrewh@myspace.com</t>
+  </si>
+  <si>
+    <t>n@gmail.com</t>
+  </si>
+  <si>
+    <t>john.cena@gmail.com</t>
+  </si>
+  <si>
     <t>johndoe</t>
   </si>
   <si>
@@ -67,6 +157,39 @@
     <t>johncena</t>
   </si>
   <si>
+    <t>sallysmith</t>
+  </si>
+  <si>
+    <t>bobcole</t>
+  </si>
+  <si>
+    <t>daviddun</t>
+  </si>
+  <si>
+    <t>emilydonald</t>
+  </si>
+  <si>
+    <t>billblah</t>
+  </si>
+  <si>
+    <t>cliftondonald</t>
+  </si>
+  <si>
+    <t>nancybryan</t>
+  </si>
+  <si>
+    <t>nevinfish</t>
+  </si>
+  <si>
+    <t>laracronin</t>
+  </si>
+  <si>
+    <t>camyrnmoltavo</t>
+  </si>
+  <si>
+    <t>nick.dw/.dww.d/.</t>
+  </si>
+  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -77,6 +200,39 @@
   </si>
   <si>
     <t>John Cena</t>
+  </si>
+  <si>
+    <t>Sally Smith</t>
+  </si>
+  <si>
+    <t>Bob Cole</t>
+  </si>
+  <si>
+    <t>David Dun</t>
+  </si>
+  <si>
+    <t>Emily Donald</t>
+  </si>
+  <si>
+    <t>Bill Blah</t>
+  </si>
+  <si>
+    <t>Clifton Donald</t>
+  </si>
+  <si>
+    <t>Nancy Bryan</t>
+  </si>
+  <si>
+    <t>Nevin Fish</t>
+  </si>
+  <si>
+    <t>Lara Cronin</t>
+  </si>
+  <si>
+    <t>Camyrn Moltavo</t>
+  </si>
+  <si>
+    <t>Nick .dw/.dww.d/.</t>
   </si>
 </sst>
 </file>
@@ -470,17 +626,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:AM16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="14" width="30.7109375" customWidth="1"/>
+    <col min="5" max="40" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,16 +676,97 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:39">
       <c r="A2">
         <v>1234567891</v>
       </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="E2">
         <f>CHOOSE(1,"","IND_OVERDUE")</f>
@@ -567,16 +804,123 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
+      <c r="N2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:39">
       <c r="A3">
         <v>3322111234</v>
       </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E3">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -614,16 +958,123 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
+      <c r="N3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f>CHOOSE(1,"2024-08-30","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <f>CHOOSE(1,"2024-08-30","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:39">
       <c r="A4">
         <v>4453245321</v>
       </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -638,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
       <c r="I4">
@@ -661,16 +1112,123 @@
         <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
         <v>0</v>
       </c>
+      <c r="N4">
+        <f>CHOOSE(1,"2022-10-30","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <f>CHOOSE(1,"2024-08-28","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:39">
       <c r="A5">
         <v>5555555555</v>
       </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
@@ -708,14 +1266,1779 @@
         <f>CHOOSE(1,"2000-01-01","IND_OVERDUE")</f>
         <v>0</v>
       </c>
+      <c r="N5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <f>CHOOSE(1,"2000-01-01","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <f>CHOOSE(1,"2000-01-01","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f>CHOOSE(1,"2020-09-01","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f>CHOOSE(1,"2024-10-15","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>CHOOSE(1,"2020-08-20","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f>CHOOSE(1,"2023-09-17","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39">
+      <c r="A9">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f>CHOOSE(1,"","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f>CHOOSE(1,"2021-05-11","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f>CHOOSE(1,"2024-10-13","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39">
+      <c r="A13">
+        <v>2000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>CHOOSE(1,"2024-06-30","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f>CHOOSE(1,"2024-10-09","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
+      <c r="A15">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>CHOOSE(1,"2023-10-23","IND_ONTIME")</f>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
+      <c r="A16">
+        <v>-1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <f>CHOOSE(1,"2024-08-28","IND_OVERDUE")</f>
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AK16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
+      <c r="AM16">
+        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E5">
+  <conditionalFormatting sqref="A2:E16">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>AND(COLUMN(A2) &lt; 5, ROW(A2) &lt; 6)</formula>
+      <formula>AND(COLUMN(A2) &lt; 5, ROW(A2) &lt; 17)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:M5">
+  <conditionalFormatting sqref="E2:AM16">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISNUMBER(SEARCH("IND_OVERDUE", _xlfn.FORMULATEXT(E2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
add source window is responsive
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>dodid</t>
   </si>
@@ -79,72 +79,9 @@
     <t>RandomCourseName2-myLearning</t>
   </si>
   <si>
-    <t>DHA Accommodations (1 hr)-badSource</t>
-  </si>
-  <si>
-    <t>Leadership Training (4 hrs)-badSource</t>
-  </si>
-  <si>
-    <t>MHS Customer Service (1 hr)-badSource</t>
-  </si>
-  <si>
-    <t>Counterintelligence (1 hr)-badSource</t>
-  </si>
-  <si>
-    <t>HIPAA Training (1 hr)-badSource</t>
-  </si>
-  <si>
-    <t>Supervisor Safety Training (2 hrs)-badSource</t>
-  </si>
-  <si>
-    <t>Employee Safety (1 hr)-badSource</t>
-  </si>
-  <si>
-    <t>Violence Response (1 hr)-badSource</t>
-  </si>
-  <si>
-    <t>RandomCourse-badSource</t>
-  </si>
-  <si>
-    <t>DHA Accommodations (1 hr)-missingID</t>
-  </si>
-  <si>
-    <t>Leadership Training (4 hrs)-missingID</t>
-  </si>
-  <si>
-    <t>MHS Customer Service (1 hr)-missingID</t>
-  </si>
-  <si>
-    <t>Counterintelligence (1 hr)-missingID</t>
-  </si>
-  <si>
-    <t>HIPAA Training (1 hr)-missingID</t>
-  </si>
-  <si>
-    <t>Supervisor Safety Training (2 hrs)-missingID</t>
-  </si>
-  <si>
-    <t>Employee Safety (1 hr)-missingID</t>
-  </si>
-  <si>
-    <t>Violence Response (1 hr)-missingID</t>
-  </si>
-  <si>
-    <t>RandomCourse-missingID</t>
-  </si>
-  <si>
-    <t>johndoe@email.com</t>
-  </si>
-  <si>
-    <t>andrewh@myspace.com</t>
-  </si>
-  <si>
     <t>n@gmail.com</t>
   </si>
   <si>
-    <t>john.cena@gmail.com</t>
-  </si>
-  <si>
     <t>johndoe</t>
   </si>
   <si>
@@ -187,9 +124,6 @@
     <t>camyrnmoltavo</t>
   </si>
   <si>
-    <t>nick.dw/.dww.d/.</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -230,9 +164,6 @@
   </si>
   <si>
     <t>Camyrn Moltavo</t>
-  </si>
-  <si>
-    <t>Nick .dw/.dww.d/.</t>
   </si>
 </sst>
 </file>
@@ -626,17 +557,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM16"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="40" width="30.7109375" customWidth="1"/>
+    <col min="5" max="22" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,73 +631,16 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:21">
       <c r="A2">
         <v>1234567891</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <f>CHOOSE(1,"","IND_OVERDUE")</f>
@@ -836,91 +710,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V2">
-        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <f>CHOOSE(1,"2024-08-31","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>3322111234</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -990,91 +789,19 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <f>CHOOSE(1,"","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <f>CHOOSE(1,"","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <f>CHOOSE(1,"2024-08-30","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <f>CHOOSE(1,"","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <f>CHOOSE(1,"","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <f>CHOOSE(1,"2024-08-30","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>4453245321</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -1144,91 +871,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <f>CHOOSE(1,"2024-08-29","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <f>CHOOSE(1,"2024-08-29","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <f>CHOOSE(1,"2024-08-28","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <f>CHOOSE(1,"2000-01-01","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>5555555555</v>
       </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
@@ -1298,88 +950,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <f>CHOOSE(1,"2000-01-01","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL5">
-        <f>CHOOSE(1,"2024-08-28","IND_ONTIME")</f>
-        <v>0</v>
-      </c>
-      <c r="AM5">
-        <f>CHOOSE(1,"2000-01-01","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -1449,88 +1029,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -1600,88 +1108,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM7">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="E8">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -1751,88 +1187,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM8">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E9">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -1902,88 +1266,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM9">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E10">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -2053,88 +1345,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM10">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -2204,88 +1424,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM11">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -2355,88 +1503,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM12">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>2000</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E13">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -2506,88 +1582,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM13">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E14">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -2657,88 +1661,16 @@
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
         <v>0</v>
       </c>
-      <c r="V14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM14">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="E15">
         <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
@@ -2808,237 +1740,14 @@
         <f>CHOOSE(1,"2023-10-23","IND_ONTIME")</f>
         <v>0</v>
       </c>
-      <c r="V15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM15">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39">
-      <c r="A16">
-        <v>-1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <f>CHOOSE(1,"2024-08-28","IND_OVERDUE")</f>
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AD16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AE16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AF16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AG16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AH16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AJ16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AK16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AL16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
-      <c r="AM16">
-        <f>CHOOSE(1,"","IND_NOTASSIGNED")</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E16">
+  <conditionalFormatting sqref="A2:E15">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>AND(COLUMN(A2) &lt; 5, ROW(A2) &lt; 17)</formula>
+      <formula>AND(COLUMN(A2) &lt; 5, ROW(A2) &lt; 16)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:AM16">
+  <conditionalFormatting sqref="E2:U15">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISNUMBER(SEARCH("IND_OVERDUE", _xlfn.FORMULATEXT(E2)))</formula>
     </cfRule>

</xml_diff>